<commit_message>
Compiled with ntis and misc
</commit_message>
<xml_diff>
--- a/data/agriculture_development_chronology.xlsx
+++ b/data/agriculture_development_chronology.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="257">
   <si>
     <t xml:space="preserve">#कृषि विकासमा कुन कहिले</t>
   </si>
@@ -802,6 +802,30 @@
   </si>
   <si>
     <t xml:space="preserve">Food management and agriculture supply corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical School at Chhauni, Kathmandu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agriculture School in Minbhawan to train JT/JTAs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagadamba College of Agriculture and Research Institute at Shreemahal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School of Agriculture at Minbhawan transformed into Maha-vidyalaya and I.Sc. Agriculture program started. The program was launched in 2027 Shrawan 26.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Maha-vidyalaya” established in 2025 converted into IAAS with affiliation of Tribhuwan University and transferred to Jagadamba building at Pulchowk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IAAS relocated to Rampur, Chitwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Sc Agriculture program started in Rampur, Chitwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhD program started in IAAS, TU</t>
   </si>
 </sst>
 </file>
@@ -911,16 +935,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D140" activeCellId="0" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.3117408906883"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
@@ -2791,6 +2815,94 @@
       </c>
       <c r="F132" s="0" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="0" t="n">
+        <v>1994</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E135" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F135" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="0" t="n">
+        <v>2025</v>
+      </c>
+      <c r="E136" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F136" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="0" t="n">
+        <v>2029</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="0" t="n">
+        <v>2030</v>
+      </c>
+      <c r="E138" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F138" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="0" t="n">
+        <v>2034</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F139" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="0" t="n">
+        <v>2059</v>
+      </c>
+      <c r="E140" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F140" s="0" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>